<commit_message>
fix(lib): missing score definition on cyfun 2025
</commit_message>
<xml_diff>
--- a/tools/excel/ccb/cyfun2025.xlsx
+++ b/tools/excel/ccb/cyfun2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/excel/ccb/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/excel/ccb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C77A99-4EB4-584B-A9DE-FE29AA3BC953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9AE6B8-4C7B-2044-8556-59D83B060D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="-28180" windowWidth="51200" windowHeight="26920" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25680" yWindow="-28020" windowWidth="25360" windowHeight="27860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="986">
   <si>
     <t>GV.OC-01.1</t>
   </si>
@@ -5719,6 +5719,21 @@
 · Training and Drills: Conduct regular training sessions and crisis simulations to ensure the team is prepared to respond effectively.
 · Monitor and Adapt: Continuously monitor the situation and adapt the communication strategy as needed to address evolving circumstances.
 · Post-Crisis Review: After the crisis, review the communication efforts to identify lessons learned and improve future responses.</t>
+  </si>
+  <si>
+    <t>min_score</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>max_score</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>scores_definition</t>
   </si>
 </sst>
 </file>
@@ -5960,7 +5975,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -5971,7 +5986,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5990,10 +6005,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6053,10 +6068,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6140,9 +6152,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -6156,13 +6165,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6471,8 +6480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5483155-6829-0140-8BF0-A0EAE8AC9D6F}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B8"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6502,7 +6511,7 @@
         <v>195</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -6575,10 +6584,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04BAF61A-04DC-E843-B98B-FBB8A932C760}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="172" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScale="254" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6643,6 +6652,30 @@
         <v>213</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>981</v>
+      </c>
+      <c r="B8" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>983</v>
+      </c>
+      <c r="B9" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>985</v>
+      </c>
+      <c r="B10" t="s">
+        <v>234</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6652,7 +6685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G335"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+    <sheetView zoomScale="173" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
@@ -8833,7 +8866,7 @@
       <c r="D126" t="s">
         <v>256</v>
       </c>
-      <c r="F126" s="35" t="s">
+      <c r="F126" s="34" t="s">
         <v>407</v>
       </c>
       <c r="G126" s="2" t="s">
@@ -8991,7 +9024,7 @@
       <c r="D136" t="s">
         <v>249</v>
       </c>
-      <c r="F136" s="37" t="s">
+      <c r="F136" s="36" t="s">
         <v>428</v>
       </c>
       <c r="G136" s="2" t="s">
@@ -9011,7 +9044,7 @@
       <c r="D137" t="s">
         <v>249</v>
       </c>
-      <c r="F137" s="36" t="s">
+      <c r="F137" s="35" t="s">
         <v>430</v>
       </c>
       <c r="G137" s="2" t="s">
@@ -9031,7 +9064,7 @@
       <c r="D138" t="s">
         <v>259</v>
       </c>
-      <c r="F138" s="36" t="s">
+      <c r="F138" s="35" t="s">
         <v>432</v>
       </c>
       <c r="G138" s="2" t="s">
@@ -9051,7 +9084,7 @@
       <c r="D139" t="s">
         <v>249</v>
       </c>
-      <c r="F139" s="36" t="s">
+      <c r="F139" s="35" t="s">
         <v>434</v>
       </c>
       <c r="G139" s="2" t="s">
@@ -9071,7 +9104,7 @@
       <c r="D140" t="s">
         <v>249</v>
       </c>
-      <c r="F140" s="36" t="s">
+      <c r="F140" s="35" t="s">
         <v>436</v>
       </c>
       <c r="G140" s="2" t="s">
@@ -9091,7 +9124,7 @@
       <c r="D141" t="s">
         <v>249</v>
       </c>
-      <c r="F141" s="36" t="s">
+      <c r="F141" s="35" t="s">
         <v>439</v>
       </c>
       <c r="G141" s="2" t="s">
@@ -9165,7 +9198,7 @@
       <c r="C145" t="s">
         <v>442</v>
       </c>
-      <c r="F145" s="36" t="s">
+      <c r="F145" s="35" t="s">
         <v>462</v>
       </c>
     </row>
@@ -9182,7 +9215,7 @@
       <c r="D146" t="s">
         <v>259</v>
       </c>
-      <c r="F146" s="36" t="s">
+      <c r="F146" s="35" t="s">
         <v>440</v>
       </c>
       <c r="G146" s="2" t="s">
@@ -9372,7 +9405,7 @@
       <c r="D157" t="s">
         <v>249</v>
       </c>
-      <c r="F157" s="38" t="s">
+      <c r="F157" s="37" t="s">
         <v>481</v>
       </c>
       <c r="G157" s="2" t="s">
@@ -9392,7 +9425,7 @@
       <c r="D158" t="s">
         <v>239</v>
       </c>
-      <c r="F158" s="39" t="s">
+      <c r="F158" s="38" t="s">
         <v>624</v>
       </c>
       <c r="G158" s="2" t="s">
@@ -9406,7 +9439,7 @@
       <c r="C159" t="s">
         <v>584</v>
       </c>
-      <c r="F159" s="39" t="s">
+      <c r="F159" s="38" t="s">
         <v>597</v>
       </c>
     </row>
@@ -9423,7 +9456,7 @@
       <c r="D160" t="s">
         <v>250</v>
       </c>
-      <c r="F160" s="39" t="s">
+      <c r="F160" s="38" t="s">
         <v>483</v>
       </c>
       <c r="G160" s="2" t="s">
@@ -9443,7 +9476,7 @@
       <c r="D161" t="s">
         <v>322</v>
       </c>
-      <c r="F161" s="40" t="s">
+      <c r="F161" s="39" t="s">
         <v>487</v>
       </c>
       <c r="G161" s="2" t="s">
@@ -9463,7 +9496,7 @@
       <c r="D162" t="s">
         <v>582</v>
       </c>
-      <c r="F162" s="41" t="s">
+      <c r="F162" s="40" t="s">
         <v>488</v>
       </c>
       <c r="G162" s="2" t="s">
@@ -9483,7 +9516,7 @@
       <c r="D163" t="s">
         <v>239</v>
       </c>
-      <c r="F163" s="63" t="s">
+      <c r="F163" s="35" t="s">
         <v>631</v>
       </c>
       <c r="G163" s="2" t="s">
@@ -9503,7 +9536,7 @@
       <c r="D164" t="s">
         <v>239</v>
       </c>
-      <c r="F164" s="63" t="s">
+      <c r="F164" s="35" t="s">
         <v>632</v>
       </c>
       <c r="G164" s="2" t="s">
@@ -9517,7 +9550,7 @@
       <c r="C165" t="s">
         <v>635</v>
       </c>
-      <c r="F165" s="63" t="s">
+      <c r="F165" s="35" t="s">
         <v>634</v>
       </c>
     </row>
@@ -9534,7 +9567,7 @@
       <c r="D166" t="s">
         <v>239</v>
       </c>
-      <c r="F166" s="63" t="s">
+      <c r="F166" s="35" t="s">
         <v>634</v>
       </c>
       <c r="G166" s="2" t="s">
@@ -9548,7 +9581,7 @@
       <c r="C167" t="s">
         <v>583</v>
       </c>
-      <c r="F167" s="63" t="s">
+      <c r="F167" s="35" t="s">
         <v>598</v>
       </c>
     </row>
@@ -9565,7 +9598,7 @@
       <c r="D168" t="s">
         <v>322</v>
       </c>
-      <c r="F168" s="42" t="s">
+      <c r="F168" s="41" t="s">
         <v>489</v>
       </c>
       <c r="G168" s="2" t="s">
@@ -9585,7 +9618,7 @@
       <c r="D169" t="s">
         <v>322</v>
       </c>
-      <c r="F169" s="40" t="s">
+      <c r="F169" s="39" t="s">
         <v>491</v>
       </c>
       <c r="G169" s="2" t="s">
@@ -9605,7 +9638,7 @@
       <c r="D170" t="s">
         <v>322</v>
       </c>
-      <c r="F170" s="43" t="s">
+      <c r="F170" s="42" t="s">
         <v>498</v>
       </c>
       <c r="G170" s="2" t="s">
@@ -9625,7 +9658,7 @@
       <c r="D171" t="s">
         <v>322</v>
       </c>
-      <c r="F171" s="41" t="s">
+      <c r="F171" s="40" t="s">
         <v>499</v>
       </c>
       <c r="G171" s="2" t="s">
@@ -9645,7 +9678,7 @@
       <c r="D172" t="s">
         <v>249</v>
       </c>
-      <c r="F172" s="37" t="s">
+      <c r="F172" s="36" t="s">
         <v>500</v>
       </c>
       <c r="G172" s="2" t="s">
@@ -9685,7 +9718,7 @@
       <c r="D174" t="s">
         <v>249</v>
       </c>
-      <c r="F174" s="44" t="s">
+      <c r="F174" s="43" t="s">
         <v>502</v>
       </c>
       <c r="G174" s="2" t="s">
@@ -9705,7 +9738,7 @@
       <c r="D175" t="s">
         <v>239</v>
       </c>
-      <c r="F175" s="61" t="s">
+      <c r="F175" s="60" t="s">
         <v>646</v>
       </c>
       <c r="G175" s="2" t="s">
@@ -9725,7 +9758,7 @@
       <c r="D176" t="s">
         <v>239</v>
       </c>
-      <c r="F176" s="61" t="s">
+      <c r="F176" s="60" t="s">
         <v>649</v>
       </c>
       <c r="G176" s="2" t="s">
@@ -9739,7 +9772,7 @@
       <c r="C177" t="s">
         <v>585</v>
       </c>
-      <c r="F177" s="61" t="s">
+      <c r="F177" s="60" t="s">
         <v>599</v>
       </c>
     </row>
@@ -9776,7 +9809,7 @@
       <c r="D179" t="s">
         <v>249</v>
       </c>
-      <c r="F179" s="45" t="s">
+      <c r="F179" s="44" t="s">
         <v>506</v>
       </c>
       <c r="G179" s="2" t="s">
@@ -9796,7 +9829,7 @@
       <c r="D180" t="s">
         <v>239</v>
       </c>
-      <c r="F180" s="62" t="s">
+      <c r="F180" s="61" t="s">
         <v>655</v>
       </c>
       <c r="G180" s="2" t="s">
@@ -9816,7 +9849,7 @@
       <c r="D181" t="s">
         <v>239</v>
       </c>
-      <c r="F181" s="62" t="s">
+      <c r="F181" s="61" t="s">
         <v>657</v>
       </c>
       <c r="G181" s="2" t="s">
@@ -9833,7 +9866,7 @@
       <c r="E182" s="5" t="s">
         <v>590</v>
       </c>
-      <c r="F182" s="62" t="s">
+      <c r="F182" s="61" t="s">
         <v>592</v>
       </c>
     </row>
@@ -9844,7 +9877,7 @@
       <c r="C183" t="s">
         <v>566</v>
       </c>
-      <c r="F183" s="62" t="s">
+      <c r="F183" s="61" t="s">
         <v>600</v>
       </c>
     </row>
@@ -9861,7 +9894,7 @@
       <c r="D184" t="s">
         <v>250</v>
       </c>
-      <c r="F184" s="46" t="s">
+      <c r="F184" s="45" t="s">
         <v>507</v>
       </c>
       <c r="G184" s="2" t="s">
@@ -9881,7 +9914,7 @@
       <c r="D185" t="s">
         <v>249</v>
       </c>
-      <c r="F185" s="58" t="s">
+      <c r="F185" s="57" t="s">
         <v>512</v>
       </c>
       <c r="G185" s="2" t="s">
@@ -9901,7 +9934,7 @@
       <c r="D186" t="s">
         <v>249</v>
       </c>
-      <c r="F186" s="57" t="s">
+      <c r="F186" s="56" t="s">
         <v>511</v>
       </c>
       <c r="G186" s="2" t="s">
@@ -10009,7 +10042,7 @@
       <c r="E192" s="5" t="s">
         <v>589</v>
       </c>
-      <c r="F192" s="36" t="s">
+      <c r="F192" s="35" t="s">
         <v>591</v>
       </c>
     </row>
@@ -10020,7 +10053,7 @@
       <c r="C193" t="s">
         <v>568</v>
       </c>
-      <c r="F193" s="36" t="s">
+      <c r="F193" s="35" t="s">
         <v>602</v>
       </c>
     </row>
@@ -10037,7 +10070,7 @@
       <c r="D194" t="s">
         <v>249</v>
       </c>
-      <c r="F194" s="47" t="s">
+      <c r="F194" s="46" t="s">
         <v>519</v>
       </c>
       <c r="G194" s="2" t="s">
@@ -10137,7 +10170,7 @@
       <c r="D199" t="s">
         <v>239</v>
       </c>
-      <c r="F199" s="64" t="s">
+      <c r="F199" s="62" t="s">
         <v>678</v>
       </c>
       <c r="G199" s="2" t="s">
@@ -10157,7 +10190,7 @@
       <c r="D200" t="s">
         <v>250</v>
       </c>
-      <c r="F200" s="48" t="s">
+      <c r="F200" s="47" t="s">
         <v>525</v>
       </c>
       <c r="G200" s="2" t="s">
@@ -10171,7 +10204,7 @@
       <c r="C201" t="s">
         <v>681</v>
       </c>
-      <c r="F201" s="36" t="s">
+      <c r="F201" s="35" t="s">
         <v>682</v>
       </c>
     </row>
@@ -10188,7 +10221,7 @@
       <c r="D202" t="s">
         <v>258</v>
       </c>
-      <c r="F202" s="36" t="s">
+      <c r="F202" s="35" t="s">
         <v>684</v>
       </c>
       <c r="G202" s="2" t="s">
@@ -10208,7 +10241,7 @@
       <c r="D203" t="s">
         <v>239</v>
       </c>
-      <c r="F203" s="36" t="s">
+      <c r="F203" s="35" t="s">
         <v>686</v>
       </c>
       <c r="G203" s="2" t="s">
@@ -10222,7 +10255,7 @@
       <c r="C204" t="s">
         <v>689</v>
       </c>
-      <c r="F204" s="36" t="s">
+      <c r="F204" s="35" t="s">
         <v>690</v>
       </c>
       <c r="G204" s="2"/>
@@ -10240,7 +10273,7 @@
       <c r="D205" t="s">
         <v>239</v>
       </c>
-      <c r="F205" s="36" t="s">
+      <c r="F205" s="35" t="s">
         <v>692</v>
       </c>
       <c r="G205" s="2" t="s">
@@ -10254,7 +10287,7 @@
       <c r="C206" t="s">
         <v>569</v>
       </c>
-      <c r="F206" s="36" t="s">
+      <c r="F206" s="35" t="s">
         <v>603</v>
       </c>
     </row>
@@ -10271,7 +10304,7 @@
       <c r="D207" t="s">
         <v>322</v>
       </c>
-      <c r="F207" s="49" t="s">
+      <c r="F207" s="48" t="s">
         <v>527</v>
       </c>
       <c r="G207" s="2" t="s">
@@ -10291,7 +10324,7 @@
       <c r="D208" t="s">
         <v>249</v>
       </c>
-      <c r="F208" s="50" t="s">
+      <c r="F208" s="49" t="s">
         <v>531</v>
       </c>
       <c r="G208" s="2" t="s">
@@ -10311,7 +10344,7 @@
       <c r="D209" t="s">
         <v>249</v>
       </c>
-      <c r="F209" s="51" t="s">
+      <c r="F209" s="50" t="s">
         <v>532</v>
       </c>
       <c r="G209" s="2" t="s">
@@ -10331,7 +10364,7 @@
       <c r="D210" t="s">
         <v>239</v>
       </c>
-      <c r="F210" s="54" t="s">
+      <c r="F210" s="53" t="s">
         <v>698</v>
       </c>
       <c r="G210" s="2" t="s">
@@ -10351,7 +10384,7 @@
       <c r="D211" t="s">
         <v>239</v>
       </c>
-      <c r="F211" s="54" t="s">
+      <c r="F211" s="53" t="s">
         <v>701</v>
       </c>
       <c r="G211" s="2" t="s">
@@ -10368,7 +10401,7 @@
       <c r="E212" s="5" t="s">
         <v>595</v>
       </c>
-      <c r="F212" s="54" t="s">
+      <c r="F212" s="53" t="s">
         <v>594</v>
       </c>
     </row>
@@ -10379,7 +10412,7 @@
       <c r="C213" t="s">
         <v>570</v>
       </c>
-      <c r="F213" s="54" t="s">
+      <c r="F213" s="53" t="s">
         <v>604</v>
       </c>
     </row>
@@ -10416,7 +10449,7 @@
       <c r="D215" t="s">
         <v>239</v>
       </c>
-      <c r="F215" s="63" t="s">
+      <c r="F215" s="35" t="s">
         <v>708</v>
       </c>
       <c r="G215" s="2" t="s">
@@ -10490,7 +10523,7 @@
       <c r="C219" t="s">
         <v>573</v>
       </c>
-      <c r="F219" s="63" t="s">
+      <c r="F219" s="35" t="s">
         <v>605</v>
       </c>
     </row>
@@ -10507,7 +10540,7 @@
       <c r="D220" t="s">
         <v>249</v>
       </c>
-      <c r="F220" s="52" t="s">
+      <c r="F220" s="51" t="s">
         <v>535</v>
       </c>
       <c r="G220" s="2" t="s">
@@ -10521,7 +10554,7 @@
       <c r="C221" t="s">
         <v>574</v>
       </c>
-      <c r="F221" s="52" t="s">
+      <c r="F221" s="51" t="s">
         <v>606</v>
       </c>
     </row>
@@ -10538,7 +10571,7 @@
       <c r="D222" t="s">
         <v>249</v>
       </c>
-      <c r="F222" s="52" t="s">
+      <c r="F222" s="51" t="s">
         <v>537</v>
       </c>
       <c r="G222" s="2" t="s">
@@ -10552,7 +10585,7 @@
       <c r="C223" t="s">
         <v>575</v>
       </c>
-      <c r="F223" s="55" t="s">
+      <c r="F223" s="54" t="s">
         <v>607</v>
       </c>
     </row>
@@ -10569,7 +10602,7 @@
       <c r="D224" t="s">
         <v>322</v>
       </c>
-      <c r="F224" s="59" t="s">
+      <c r="F224" s="58" t="s">
         <v>539</v>
       </c>
       <c r="G224" s="2" t="s">
@@ -10589,7 +10622,7 @@
       <c r="D225" t="s">
         <v>249</v>
       </c>
-      <c r="F225" s="53" t="s">
+      <c r="F225" s="52" t="s">
         <v>544</v>
       </c>
       <c r="G225" s="2" t="s">
@@ -10609,7 +10642,7 @@
       <c r="D226" t="s">
         <v>249</v>
       </c>
-      <c r="F226" s="54" t="s">
+      <c r="F226" s="53" t="s">
         <v>543</v>
       </c>
       <c r="G226" s="2" t="s">
@@ -10663,7 +10696,7 @@
       <c r="C229" t="s">
         <v>576</v>
       </c>
-      <c r="F229" s="50" t="s">
+      <c r="F229" s="49" t="s">
         <v>608</v>
       </c>
     </row>
@@ -10680,7 +10713,7 @@
       <c r="D230" t="s">
         <v>250</v>
       </c>
-      <c r="F230" s="55" t="s">
+      <c r="F230" s="54" t="s">
         <v>545</v>
       </c>
       <c r="G230" s="2" t="s">
@@ -10700,7 +10733,7 @@
       <c r="D231" t="s">
         <v>249</v>
       </c>
-      <c r="F231" s="51" t="s">
+      <c r="F231" s="50" t="s">
         <v>548</v>
       </c>
       <c r="G231" s="2" t="s">
@@ -10714,7 +10747,7 @@
       <c r="C232" t="s">
         <v>577</v>
       </c>
-      <c r="F232" s="50" t="s">
+      <c r="F232" s="49" t="s">
         <v>609</v>
       </c>
     </row>
@@ -10731,7 +10764,7 @@
       <c r="D233" t="s">
         <v>249</v>
       </c>
-      <c r="F233" s="55" t="s">
+      <c r="F233" s="54" t="s">
         <v>549</v>
       </c>
       <c r="G233" s="2" t="s">
@@ -10751,7 +10784,7 @@
       <c r="D234" t="s">
         <v>249</v>
       </c>
-      <c r="F234" s="51" t="s">
+      <c r="F234" s="50" t="s">
         <v>551</v>
       </c>
       <c r="G234" s="2" t="s">
@@ -10771,7 +10804,7 @@
       <c r="D235" t="s">
         <v>239</v>
       </c>
-      <c r="F235" s="50" t="s">
+      <c r="F235" s="49" t="s">
         <v>733</v>
       </c>
       <c r="G235" s="2" t="s">
@@ -10808,7 +10841,7 @@
       <c r="E237" s="5" t="s">
         <v>588</v>
       </c>
-      <c r="F237" s="50" t="s">
+      <c r="F237" s="49" t="s">
         <v>587</v>
       </c>
     </row>
@@ -10819,7 +10852,7 @@
       <c r="C238" t="s">
         <v>578</v>
       </c>
-      <c r="F238" s="50" t="s">
+      <c r="F238" s="49" t="s">
         <v>610</v>
       </c>
     </row>
@@ -10836,7 +10869,7 @@
       <c r="D239" t="s">
         <v>322</v>
       </c>
-      <c r="F239" s="49" t="s">
+      <c r="F239" s="48" t="s">
         <v>553</v>
       </c>
       <c r="G239" s="2" t="s">
@@ -10856,7 +10889,7 @@
       <c r="D240" t="s">
         <v>322</v>
       </c>
-      <c r="F240" s="56" t="s">
+      <c r="F240" s="55" t="s">
         <v>555</v>
       </c>
       <c r="G240" s="2" t="s">
@@ -10876,7 +10909,7 @@
       <c r="D241" t="s">
         <v>582</v>
       </c>
-      <c r="F241" s="40" t="s">
+      <c r="F241" s="39" t="s">
         <v>559</v>
       </c>
       <c r="G241" s="2" t="s">
@@ -10896,7 +10929,7 @@
       <c r="D242" t="s">
         <v>582</v>
       </c>
-      <c r="F242" s="41" t="s">
+      <c r="F242" s="40" t="s">
         <v>560</v>
       </c>
       <c r="G242" s="2" t="s">
@@ -11010,7 +11043,7 @@
       <c r="C248" t="s">
         <v>580</v>
       </c>
-      <c r="F248" s="63" t="s">
+      <c r="F248" s="35" t="s">
         <v>611</v>
       </c>
     </row>
@@ -11027,7 +11060,7 @@
       <c r="D249" t="s">
         <v>249</v>
       </c>
-      <c r="F249" s="52" t="s">
+      <c r="F249" s="51" t="s">
         <v>561</v>
       </c>
       <c r="G249" s="2" t="s">
@@ -11047,7 +11080,7 @@
       <c r="D250" t="s">
         <v>239</v>
       </c>
-      <c r="F250" s="52" t="s">
+      <c r="F250" s="51" t="s">
         <v>758</v>
       </c>
       <c r="G250" s="2" t="s">
@@ -11061,7 +11094,7 @@
       <c r="C251" t="s">
         <v>760</v>
       </c>
-      <c r="F251" s="52" t="s">
+      <c r="F251" s="51" t="s">
         <v>765</v>
       </c>
       <c r="G251" s="2"/>
@@ -11093,7 +11126,7 @@
       <c r="C253" t="s">
         <v>581</v>
       </c>
-      <c r="F253" s="52" t="s">
+      <c r="F253" s="51" t="s">
         <v>612</v>
       </c>
     </row>
@@ -11110,7 +11143,7 @@
       <c r="D254" t="s">
         <v>249</v>
       </c>
-      <c r="F254" s="52" t="s">
+      <c r="F254" s="51" t="s">
         <v>563</v>
       </c>
       <c r="G254" s="2" t="s">
@@ -11152,7 +11185,7 @@
         <v>770</v>
       </c>
       <c r="E257" s="2"/>
-      <c r="F257" s="34" t="s">
+      <c r="F257" s="2" t="s">
         <v>774</v>
       </c>
     </row>
@@ -11169,7 +11202,7 @@
       <c r="D258" t="s">
         <v>250</v>
       </c>
-      <c r="F258" s="39" t="s">
+      <c r="F258" s="38" t="s">
         <v>820</v>
       </c>
       <c r="G258" s="2" t="s">
@@ -11189,7 +11222,7 @@
       <c r="D259" t="s">
         <v>322</v>
       </c>
-      <c r="F259" s="65" t="s">
+      <c r="F259" s="63" t="s">
         <v>821</v>
       </c>
       <c r="G259" s="2" t="s">
@@ -11209,7 +11242,7 @@
       <c r="D260" t="s">
         <v>582</v>
       </c>
-      <c r="F260" s="60" t="s">
+      <c r="F260" s="59" t="s">
         <v>822</v>
       </c>
       <c r="G260" s="2" t="s">
@@ -11311,7 +11344,7 @@
       <c r="D266" t="s">
         <v>250</v>
       </c>
-      <c r="F266" s="39" t="s">
+      <c r="F266" s="38" t="s">
         <v>783</v>
       </c>
       <c r="G266" s="2" t="s">
@@ -11331,7 +11364,7 @@
       <c r="D267" t="s">
         <v>249</v>
       </c>
-      <c r="F267" s="66" t="s">
+      <c r="F267" s="64" t="s">
         <v>786</v>
       </c>
       <c r="G267" s="2" t="s">
@@ -11353,7 +11386,7 @@
       <c r="A269" t="s">
         <v>126</v>
       </c>
-      <c r="B269" s="68">
+      <c r="B269" s="66">
         <v>4</v>
       </c>
       <c r="C269" t="s">
@@ -11362,7 +11395,7 @@
       <c r="D269" t="s">
         <v>249</v>
       </c>
-      <c r="F269" s="37" t="s">
+      <c r="F269" s="36" t="s">
         <v>789</v>
       </c>
       <c r="G269" s="2" t="s">
@@ -11373,7 +11406,7 @@
       <c r="A270" t="s">
         <v>126</v>
       </c>
-      <c r="B270" s="68">
+      <c r="B270" s="66">
         <v>4</v>
       </c>
       <c r="C270" t="s">
@@ -11382,7 +11415,7 @@
       <c r="D270" t="s">
         <v>249</v>
       </c>
-      <c r="F270" s="67" t="s">
+      <c r="F270" s="65" t="s">
         <v>792</v>
       </c>
       <c r="G270" s="2" t="s">
@@ -11569,7 +11602,7 @@
       <c r="D281" t="s">
         <v>322</v>
       </c>
-      <c r="F281" s="59" t="s">
+      <c r="F281" s="58" t="s">
         <v>806</v>
       </c>
       <c r="G281" s="2" t="s">
@@ -11589,7 +11622,7 @@
       <c r="D282" t="s">
         <v>249</v>
       </c>
-      <c r="F282" s="67" t="s">
+      <c r="F282" s="65" t="s">
         <v>809</v>
       </c>
       <c r="G282" s="2" t="s">
@@ -11623,7 +11656,7 @@
       <c r="C284" t="s">
         <v>817</v>
       </c>
-      <c r="F284" s="69" t="s">
+      <c r="F284" s="67" t="s">
         <v>818</v>
       </c>
     </row>
@@ -11640,7 +11673,7 @@
       <c r="D285" t="s">
         <v>256</v>
       </c>
-      <c r="F285" s="69" t="s">
+      <c r="F285" s="67" t="s">
         <v>858</v>
       </c>
       <c r="G285" s="2" t="s">
@@ -11760,7 +11793,7 @@
       <c r="D293" t="s">
         <v>250</v>
       </c>
-      <c r="F293" s="39" t="s">
+      <c r="F293" s="38" t="s">
         <v>868</v>
       </c>
       <c r="G293" s="2" t="s">
@@ -11780,7 +11813,7 @@
       <c r="D294" t="s">
         <v>249</v>
       </c>
-      <c r="F294" s="66" t="s">
+      <c r="F294" s="64" t="s">
         <v>871</v>
       </c>
       <c r="G294" s="2" t="s">
@@ -11811,7 +11844,7 @@
       <c r="D296" t="s">
         <v>249</v>
       </c>
-      <c r="F296" s="47" t="s">
+      <c r="F296" s="46" t="s">
         <v>874</v>
       </c>
       <c r="G296" s="2" t="s">
@@ -11831,7 +11864,7 @@
       <c r="D297" t="s">
         <v>239</v>
       </c>
-      <c r="F297" s="39" t="s">
+      <c r="F297" s="38" t="s">
         <v>904</v>
       </c>
       <c r="G297" s="2" t="s">
@@ -11845,7 +11878,7 @@
       <c r="C298" t="s">
         <v>877</v>
       </c>
-      <c r="F298" s="39" t="s">
+      <c r="F298" s="38" t="s">
         <v>876</v>
       </c>
     </row>
@@ -11862,7 +11895,7 @@
       <c r="D299" t="s">
         <v>249</v>
       </c>
-      <c r="F299" s="38" t="s">
+      <c r="F299" s="37" t="s">
         <v>907</v>
       </c>
       <c r="G299" s="2" t="s">
@@ -11876,7 +11909,7 @@
       <c r="C300" t="s">
         <v>880</v>
       </c>
-      <c r="F300" s="38" t="s">
+      <c r="F300" s="37" t="s">
         <v>879</v>
       </c>
     </row>
@@ -11893,7 +11926,7 @@
       <c r="D301" t="s">
         <v>249</v>
       </c>
-      <c r="F301" s="38" t="s">
+      <c r="F301" s="37" t="s">
         <v>881</v>
       </c>
       <c r="G301" s="2" t="s">
@@ -11907,7 +11940,7 @@
       <c r="C302" t="s">
         <v>910</v>
       </c>
-      <c r="E302" s="71" t="s">
+      <c r="E302" s="69" t="s">
         <v>911</v>
       </c>
       <c r="F302" s="2" t="s">
@@ -11922,7 +11955,7 @@
       <c r="C303" t="s">
         <v>914</v>
       </c>
-      <c r="E303" s="71"/>
+      <c r="E303" s="69"/>
       <c r="F303" s="2" t="s">
         <v>913</v>
       </c>
@@ -11941,7 +11974,7 @@
       <c r="D304" t="s">
         <v>239</v>
       </c>
-      <c r="E304" s="71"/>
+      <c r="E304" s="69"/>
       <c r="F304" s="2" t="s">
         <v>915</v>
       </c>
@@ -11956,7 +11989,7 @@
       <c r="C305" t="s">
         <v>918</v>
       </c>
-      <c r="E305" s="71"/>
+      <c r="E305" s="69"/>
       <c r="F305" s="2" t="s">
         <v>919</v>
       </c>
@@ -11975,7 +12008,7 @@
       <c r="D306" t="s">
         <v>239</v>
       </c>
-      <c r="E306" s="71"/>
+      <c r="E306" s="69"/>
       <c r="F306" s="2" t="s">
         <v>921</v>
       </c>
@@ -11990,7 +12023,7 @@
       <c r="C307" t="s">
         <v>923</v>
       </c>
-      <c r="E307" s="71"/>
+      <c r="E307" s="69"/>
       <c r="F307" s="2" t="s">
         <v>924</v>
       </c>
@@ -12009,7 +12042,7 @@
       <c r="D308" t="s">
         <v>239</v>
       </c>
-      <c r="E308" s="71"/>
+      <c r="E308" s="69"/>
       <c r="F308" s="2" t="s">
         <v>925</v>
       </c>
@@ -12024,7 +12057,7 @@
       <c r="C309" t="s">
         <v>929</v>
       </c>
-      <c r="E309" s="71"/>
+      <c r="E309" s="69"/>
       <c r="F309" s="2" t="s">
         <v>928</v>
       </c>
@@ -12043,7 +12076,7 @@
       <c r="D310" t="s">
         <v>239</v>
       </c>
-      <c r="E310" s="71"/>
+      <c r="E310" s="69"/>
       <c r="F310" s="2" t="s">
         <v>930</v>
       </c>
@@ -12089,7 +12122,7 @@
       <c r="D313" t="s">
         <v>250</v>
       </c>
-      <c r="F313" s="39" t="s">
+      <c r="F313" s="38" t="s">
         <v>888</v>
       </c>
       <c r="G313" s="2" t="s">
@@ -12109,7 +12142,7 @@
       <c r="D314" t="s">
         <v>582</v>
       </c>
-      <c r="F314" s="70" t="s">
+      <c r="F314" s="68" t="s">
         <v>891</v>
       </c>
       <c r="G314" s="2" t="s">
@@ -12154,7 +12187,7 @@
       <c r="D317" t="s">
         <v>249</v>
       </c>
-      <c r="F317" s="36" t="s">
+      <c r="F317" s="35" t="s">
         <v>897</v>
       </c>
       <c r="G317" s="2" t="s">
@@ -12174,7 +12207,7 @@
       <c r="D318" t="s">
         <v>582</v>
       </c>
-      <c r="F318" s="70" t="s">
+      <c r="F318" s="68" t="s">
         <v>900</v>
       </c>
       <c r="G318" s="2" t="s">
@@ -12631,7 +12664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{242BF215-323D-D147-A6AA-4FC77FB34358}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
+    <sheetView zoomScale="168" workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix(lib): missing score definition on cyfun 2025 (#2741)
</commit_message>
<xml_diff>
--- a/tools/excel/ccb/cyfun2025.xlsx
+++ b/tools/excel/ccb/cyfun2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/excel/ccb/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/excel/ccb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C77A99-4EB4-584B-A9DE-FE29AA3BC953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9AE6B8-4C7B-2044-8556-59D83B060D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="-28180" windowWidth="51200" windowHeight="26920" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25680" yWindow="-28020" windowWidth="25360" windowHeight="27860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="986">
   <si>
     <t>GV.OC-01.1</t>
   </si>
@@ -5719,6 +5719,21 @@
 · Training and Drills: Conduct regular training sessions and crisis simulations to ensure the team is prepared to respond effectively.
 · Monitor and Adapt: Continuously monitor the situation and adapt the communication strategy as needed to address evolving circumstances.
 · Post-Crisis Review: After the crisis, review the communication efforts to identify lessons learned and improve future responses.</t>
+  </si>
+  <si>
+    <t>min_score</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>max_score</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>scores_definition</t>
   </si>
 </sst>
 </file>
@@ -5960,7 +5975,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -5971,7 +5986,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5990,10 +6005,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6053,10 +6068,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6140,9 +6152,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -6156,13 +6165,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6471,8 +6480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5483155-6829-0140-8BF0-A0EAE8AC9D6F}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B8"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6502,7 +6511,7 @@
         <v>195</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -6575,10 +6584,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04BAF61A-04DC-E843-B98B-FBB8A932C760}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="172" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScale="254" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6643,6 +6652,30 @@
         <v>213</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>981</v>
+      </c>
+      <c r="B8" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>983</v>
+      </c>
+      <c r="B9" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>985</v>
+      </c>
+      <c r="B10" t="s">
+        <v>234</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6652,7 +6685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G335"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+    <sheetView zoomScale="173" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
@@ -8833,7 +8866,7 @@
       <c r="D126" t="s">
         <v>256</v>
       </c>
-      <c r="F126" s="35" t="s">
+      <c r="F126" s="34" t="s">
         <v>407</v>
       </c>
       <c r="G126" s="2" t="s">
@@ -8991,7 +9024,7 @@
       <c r="D136" t="s">
         <v>249</v>
       </c>
-      <c r="F136" s="37" t="s">
+      <c r="F136" s="36" t="s">
         <v>428</v>
       </c>
       <c r="G136" s="2" t="s">
@@ -9011,7 +9044,7 @@
       <c r="D137" t="s">
         <v>249</v>
       </c>
-      <c r="F137" s="36" t="s">
+      <c r="F137" s="35" t="s">
         <v>430</v>
       </c>
       <c r="G137" s="2" t="s">
@@ -9031,7 +9064,7 @@
       <c r="D138" t="s">
         <v>259</v>
       </c>
-      <c r="F138" s="36" t="s">
+      <c r="F138" s="35" t="s">
         <v>432</v>
       </c>
       <c r="G138" s="2" t="s">
@@ -9051,7 +9084,7 @@
       <c r="D139" t="s">
         <v>249</v>
       </c>
-      <c r="F139" s="36" t="s">
+      <c r="F139" s="35" t="s">
         <v>434</v>
       </c>
       <c r="G139" s="2" t="s">
@@ -9071,7 +9104,7 @@
       <c r="D140" t="s">
         <v>249</v>
       </c>
-      <c r="F140" s="36" t="s">
+      <c r="F140" s="35" t="s">
         <v>436</v>
       </c>
       <c r="G140" s="2" t="s">
@@ -9091,7 +9124,7 @@
       <c r="D141" t="s">
         <v>249</v>
       </c>
-      <c r="F141" s="36" t="s">
+      <c r="F141" s="35" t="s">
         <v>439</v>
       </c>
       <c r="G141" s="2" t="s">
@@ -9165,7 +9198,7 @@
       <c r="C145" t="s">
         <v>442</v>
       </c>
-      <c r="F145" s="36" t="s">
+      <c r="F145" s="35" t="s">
         <v>462</v>
       </c>
     </row>
@@ -9182,7 +9215,7 @@
       <c r="D146" t="s">
         <v>259</v>
       </c>
-      <c r="F146" s="36" t="s">
+      <c r="F146" s="35" t="s">
         <v>440</v>
       </c>
       <c r="G146" s="2" t="s">
@@ -9372,7 +9405,7 @@
       <c r="D157" t="s">
         <v>249</v>
       </c>
-      <c r="F157" s="38" t="s">
+      <c r="F157" s="37" t="s">
         <v>481</v>
       </c>
       <c r="G157" s="2" t="s">
@@ -9392,7 +9425,7 @@
       <c r="D158" t="s">
         <v>239</v>
       </c>
-      <c r="F158" s="39" t="s">
+      <c r="F158" s="38" t="s">
         <v>624</v>
       </c>
       <c r="G158" s="2" t="s">
@@ -9406,7 +9439,7 @@
       <c r="C159" t="s">
         <v>584</v>
       </c>
-      <c r="F159" s="39" t="s">
+      <c r="F159" s="38" t="s">
         <v>597</v>
       </c>
     </row>
@@ -9423,7 +9456,7 @@
       <c r="D160" t="s">
         <v>250</v>
       </c>
-      <c r="F160" s="39" t="s">
+      <c r="F160" s="38" t="s">
         <v>483</v>
       </c>
       <c r="G160" s="2" t="s">
@@ -9443,7 +9476,7 @@
       <c r="D161" t="s">
         <v>322</v>
       </c>
-      <c r="F161" s="40" t="s">
+      <c r="F161" s="39" t="s">
         <v>487</v>
       </c>
       <c r="G161" s="2" t="s">
@@ -9463,7 +9496,7 @@
       <c r="D162" t="s">
         <v>582</v>
       </c>
-      <c r="F162" s="41" t="s">
+      <c r="F162" s="40" t="s">
         <v>488</v>
       </c>
       <c r="G162" s="2" t="s">
@@ -9483,7 +9516,7 @@
       <c r="D163" t="s">
         <v>239</v>
       </c>
-      <c r="F163" s="63" t="s">
+      <c r="F163" s="35" t="s">
         <v>631</v>
       </c>
       <c r="G163" s="2" t="s">
@@ -9503,7 +9536,7 @@
       <c r="D164" t="s">
         <v>239</v>
       </c>
-      <c r="F164" s="63" t="s">
+      <c r="F164" s="35" t="s">
         <v>632</v>
       </c>
       <c r="G164" s="2" t="s">
@@ -9517,7 +9550,7 @@
       <c r="C165" t="s">
         <v>635</v>
       </c>
-      <c r="F165" s="63" t="s">
+      <c r="F165" s="35" t="s">
         <v>634</v>
       </c>
     </row>
@@ -9534,7 +9567,7 @@
       <c r="D166" t="s">
         <v>239</v>
       </c>
-      <c r="F166" s="63" t="s">
+      <c r="F166" s="35" t="s">
         <v>634</v>
       </c>
       <c r="G166" s="2" t="s">
@@ -9548,7 +9581,7 @@
       <c r="C167" t="s">
         <v>583</v>
       </c>
-      <c r="F167" s="63" t="s">
+      <c r="F167" s="35" t="s">
         <v>598</v>
       </c>
     </row>
@@ -9565,7 +9598,7 @@
       <c r="D168" t="s">
         <v>322</v>
       </c>
-      <c r="F168" s="42" t="s">
+      <c r="F168" s="41" t="s">
         <v>489</v>
       </c>
       <c r="G168" s="2" t="s">
@@ -9585,7 +9618,7 @@
       <c r="D169" t="s">
         <v>322</v>
       </c>
-      <c r="F169" s="40" t="s">
+      <c r="F169" s="39" t="s">
         <v>491</v>
       </c>
       <c r="G169" s="2" t="s">
@@ -9605,7 +9638,7 @@
       <c r="D170" t="s">
         <v>322</v>
       </c>
-      <c r="F170" s="43" t="s">
+      <c r="F170" s="42" t="s">
         <v>498</v>
       </c>
       <c r="G170" s="2" t="s">
@@ -9625,7 +9658,7 @@
       <c r="D171" t="s">
         <v>322</v>
       </c>
-      <c r="F171" s="41" t="s">
+      <c r="F171" s="40" t="s">
         <v>499</v>
       </c>
       <c r="G171" s="2" t="s">
@@ -9645,7 +9678,7 @@
       <c r="D172" t="s">
         <v>249</v>
       </c>
-      <c r="F172" s="37" t="s">
+      <c r="F172" s="36" t="s">
         <v>500</v>
       </c>
       <c r="G172" s="2" t="s">
@@ -9685,7 +9718,7 @@
       <c r="D174" t="s">
         <v>249</v>
       </c>
-      <c r="F174" s="44" t="s">
+      <c r="F174" s="43" t="s">
         <v>502</v>
       </c>
       <c r="G174" s="2" t="s">
@@ -9705,7 +9738,7 @@
       <c r="D175" t="s">
         <v>239</v>
       </c>
-      <c r="F175" s="61" t="s">
+      <c r="F175" s="60" t="s">
         <v>646</v>
       </c>
       <c r="G175" s="2" t="s">
@@ -9725,7 +9758,7 @@
       <c r="D176" t="s">
         <v>239</v>
       </c>
-      <c r="F176" s="61" t="s">
+      <c r="F176" s="60" t="s">
         <v>649</v>
       </c>
       <c r="G176" s="2" t="s">
@@ -9739,7 +9772,7 @@
       <c r="C177" t="s">
         <v>585</v>
       </c>
-      <c r="F177" s="61" t="s">
+      <c r="F177" s="60" t="s">
         <v>599</v>
       </c>
     </row>
@@ -9776,7 +9809,7 @@
       <c r="D179" t="s">
         <v>249</v>
       </c>
-      <c r="F179" s="45" t="s">
+      <c r="F179" s="44" t="s">
         <v>506</v>
       </c>
       <c r="G179" s="2" t="s">
@@ -9796,7 +9829,7 @@
       <c r="D180" t="s">
         <v>239</v>
       </c>
-      <c r="F180" s="62" t="s">
+      <c r="F180" s="61" t="s">
         <v>655</v>
       </c>
       <c r="G180" s="2" t="s">
@@ -9816,7 +9849,7 @@
       <c r="D181" t="s">
         <v>239</v>
       </c>
-      <c r="F181" s="62" t="s">
+      <c r="F181" s="61" t="s">
         <v>657</v>
       </c>
       <c r="G181" s="2" t="s">
@@ -9833,7 +9866,7 @@
       <c r="E182" s="5" t="s">
         <v>590</v>
       </c>
-      <c r="F182" s="62" t="s">
+      <c r="F182" s="61" t="s">
         <v>592</v>
       </c>
     </row>
@@ -9844,7 +9877,7 @@
       <c r="C183" t="s">
         <v>566</v>
       </c>
-      <c r="F183" s="62" t="s">
+      <c r="F183" s="61" t="s">
         <v>600</v>
       </c>
     </row>
@@ -9861,7 +9894,7 @@
       <c r="D184" t="s">
         <v>250</v>
       </c>
-      <c r="F184" s="46" t="s">
+      <c r="F184" s="45" t="s">
         <v>507</v>
       </c>
       <c r="G184" s="2" t="s">
@@ -9881,7 +9914,7 @@
       <c r="D185" t="s">
         <v>249</v>
       </c>
-      <c r="F185" s="58" t="s">
+      <c r="F185" s="57" t="s">
         <v>512</v>
       </c>
       <c r="G185" s="2" t="s">
@@ -9901,7 +9934,7 @@
       <c r="D186" t="s">
         <v>249</v>
       </c>
-      <c r="F186" s="57" t="s">
+      <c r="F186" s="56" t="s">
         <v>511</v>
       </c>
       <c r="G186" s="2" t="s">
@@ -10009,7 +10042,7 @@
       <c r="E192" s="5" t="s">
         <v>589</v>
       </c>
-      <c r="F192" s="36" t="s">
+      <c r="F192" s="35" t="s">
         <v>591</v>
       </c>
     </row>
@@ -10020,7 +10053,7 @@
       <c r="C193" t="s">
         <v>568</v>
       </c>
-      <c r="F193" s="36" t="s">
+      <c r="F193" s="35" t="s">
         <v>602</v>
       </c>
     </row>
@@ -10037,7 +10070,7 @@
       <c r="D194" t="s">
         <v>249</v>
       </c>
-      <c r="F194" s="47" t="s">
+      <c r="F194" s="46" t="s">
         <v>519</v>
       </c>
       <c r="G194" s="2" t="s">
@@ -10137,7 +10170,7 @@
       <c r="D199" t="s">
         <v>239</v>
       </c>
-      <c r="F199" s="64" t="s">
+      <c r="F199" s="62" t="s">
         <v>678</v>
       </c>
       <c r="G199" s="2" t="s">
@@ -10157,7 +10190,7 @@
       <c r="D200" t="s">
         <v>250</v>
       </c>
-      <c r="F200" s="48" t="s">
+      <c r="F200" s="47" t="s">
         <v>525</v>
       </c>
       <c r="G200" s="2" t="s">
@@ -10171,7 +10204,7 @@
       <c r="C201" t="s">
         <v>681</v>
       </c>
-      <c r="F201" s="36" t="s">
+      <c r="F201" s="35" t="s">
         <v>682</v>
       </c>
     </row>
@@ -10188,7 +10221,7 @@
       <c r="D202" t="s">
         <v>258</v>
       </c>
-      <c r="F202" s="36" t="s">
+      <c r="F202" s="35" t="s">
         <v>684</v>
       </c>
       <c r="G202" s="2" t="s">
@@ -10208,7 +10241,7 @@
       <c r="D203" t="s">
         <v>239</v>
       </c>
-      <c r="F203" s="36" t="s">
+      <c r="F203" s="35" t="s">
         <v>686</v>
       </c>
       <c r="G203" s="2" t="s">
@@ -10222,7 +10255,7 @@
       <c r="C204" t="s">
         <v>689</v>
       </c>
-      <c r="F204" s="36" t="s">
+      <c r="F204" s="35" t="s">
         <v>690</v>
       </c>
       <c r="G204" s="2"/>
@@ -10240,7 +10273,7 @@
       <c r="D205" t="s">
         <v>239</v>
       </c>
-      <c r="F205" s="36" t="s">
+      <c r="F205" s="35" t="s">
         <v>692</v>
       </c>
       <c r="G205" s="2" t="s">
@@ -10254,7 +10287,7 @@
       <c r="C206" t="s">
         <v>569</v>
       </c>
-      <c r="F206" s="36" t="s">
+      <c r="F206" s="35" t="s">
         <v>603</v>
       </c>
     </row>
@@ -10271,7 +10304,7 @@
       <c r="D207" t="s">
         <v>322</v>
       </c>
-      <c r="F207" s="49" t="s">
+      <c r="F207" s="48" t="s">
         <v>527</v>
       </c>
       <c r="G207" s="2" t="s">
@@ -10291,7 +10324,7 @@
       <c r="D208" t="s">
         <v>249</v>
       </c>
-      <c r="F208" s="50" t="s">
+      <c r="F208" s="49" t="s">
         <v>531</v>
       </c>
       <c r="G208" s="2" t="s">
@@ -10311,7 +10344,7 @@
       <c r="D209" t="s">
         <v>249</v>
       </c>
-      <c r="F209" s="51" t="s">
+      <c r="F209" s="50" t="s">
         <v>532</v>
       </c>
       <c r="G209" s="2" t="s">
@@ -10331,7 +10364,7 @@
       <c r="D210" t="s">
         <v>239</v>
       </c>
-      <c r="F210" s="54" t="s">
+      <c r="F210" s="53" t="s">
         <v>698</v>
       </c>
       <c r="G210" s="2" t="s">
@@ -10351,7 +10384,7 @@
       <c r="D211" t="s">
         <v>239</v>
       </c>
-      <c r="F211" s="54" t="s">
+      <c r="F211" s="53" t="s">
         <v>701</v>
       </c>
       <c r="G211" s="2" t="s">
@@ -10368,7 +10401,7 @@
       <c r="E212" s="5" t="s">
         <v>595</v>
       </c>
-      <c r="F212" s="54" t="s">
+      <c r="F212" s="53" t="s">
         <v>594</v>
       </c>
     </row>
@@ -10379,7 +10412,7 @@
       <c r="C213" t="s">
         <v>570</v>
       </c>
-      <c r="F213" s="54" t="s">
+      <c r="F213" s="53" t="s">
         <v>604</v>
       </c>
     </row>
@@ -10416,7 +10449,7 @@
       <c r="D215" t="s">
         <v>239</v>
       </c>
-      <c r="F215" s="63" t="s">
+      <c r="F215" s="35" t="s">
         <v>708</v>
       </c>
       <c r="G215" s="2" t="s">
@@ -10490,7 +10523,7 @@
       <c r="C219" t="s">
         <v>573</v>
       </c>
-      <c r="F219" s="63" t="s">
+      <c r="F219" s="35" t="s">
         <v>605</v>
       </c>
     </row>
@@ -10507,7 +10540,7 @@
       <c r="D220" t="s">
         <v>249</v>
       </c>
-      <c r="F220" s="52" t="s">
+      <c r="F220" s="51" t="s">
         <v>535</v>
       </c>
       <c r="G220" s="2" t="s">
@@ -10521,7 +10554,7 @@
       <c r="C221" t="s">
         <v>574</v>
       </c>
-      <c r="F221" s="52" t="s">
+      <c r="F221" s="51" t="s">
         <v>606</v>
       </c>
     </row>
@@ -10538,7 +10571,7 @@
       <c r="D222" t="s">
         <v>249</v>
       </c>
-      <c r="F222" s="52" t="s">
+      <c r="F222" s="51" t="s">
         <v>537</v>
       </c>
       <c r="G222" s="2" t="s">
@@ -10552,7 +10585,7 @@
       <c r="C223" t="s">
         <v>575</v>
       </c>
-      <c r="F223" s="55" t="s">
+      <c r="F223" s="54" t="s">
         <v>607</v>
       </c>
     </row>
@@ -10569,7 +10602,7 @@
       <c r="D224" t="s">
         <v>322</v>
       </c>
-      <c r="F224" s="59" t="s">
+      <c r="F224" s="58" t="s">
         <v>539</v>
       </c>
       <c r="G224" s="2" t="s">
@@ -10589,7 +10622,7 @@
       <c r="D225" t="s">
         <v>249</v>
       </c>
-      <c r="F225" s="53" t="s">
+      <c r="F225" s="52" t="s">
         <v>544</v>
       </c>
       <c r="G225" s="2" t="s">
@@ -10609,7 +10642,7 @@
       <c r="D226" t="s">
         <v>249</v>
       </c>
-      <c r="F226" s="54" t="s">
+      <c r="F226" s="53" t="s">
         <v>543</v>
       </c>
       <c r="G226" s="2" t="s">
@@ -10663,7 +10696,7 @@
       <c r="C229" t="s">
         <v>576</v>
       </c>
-      <c r="F229" s="50" t="s">
+      <c r="F229" s="49" t="s">
         <v>608</v>
       </c>
     </row>
@@ -10680,7 +10713,7 @@
       <c r="D230" t="s">
         <v>250</v>
       </c>
-      <c r="F230" s="55" t="s">
+      <c r="F230" s="54" t="s">
         <v>545</v>
       </c>
       <c r="G230" s="2" t="s">
@@ -10700,7 +10733,7 @@
       <c r="D231" t="s">
         <v>249</v>
       </c>
-      <c r="F231" s="51" t="s">
+      <c r="F231" s="50" t="s">
         <v>548</v>
       </c>
       <c r="G231" s="2" t="s">
@@ -10714,7 +10747,7 @@
       <c r="C232" t="s">
         <v>577</v>
       </c>
-      <c r="F232" s="50" t="s">
+      <c r="F232" s="49" t="s">
         <v>609</v>
       </c>
     </row>
@@ -10731,7 +10764,7 @@
       <c r="D233" t="s">
         <v>249</v>
       </c>
-      <c r="F233" s="55" t="s">
+      <c r="F233" s="54" t="s">
         <v>549</v>
       </c>
       <c r="G233" s="2" t="s">
@@ -10751,7 +10784,7 @@
       <c r="D234" t="s">
         <v>249</v>
       </c>
-      <c r="F234" s="51" t="s">
+      <c r="F234" s="50" t="s">
         <v>551</v>
       </c>
       <c r="G234" s="2" t="s">
@@ -10771,7 +10804,7 @@
       <c r="D235" t="s">
         <v>239</v>
       </c>
-      <c r="F235" s="50" t="s">
+      <c r="F235" s="49" t="s">
         <v>733</v>
       </c>
       <c r="G235" s="2" t="s">
@@ -10808,7 +10841,7 @@
       <c r="E237" s="5" t="s">
         <v>588</v>
       </c>
-      <c r="F237" s="50" t="s">
+      <c r="F237" s="49" t="s">
         <v>587</v>
       </c>
     </row>
@@ -10819,7 +10852,7 @@
       <c r="C238" t="s">
         <v>578</v>
       </c>
-      <c r="F238" s="50" t="s">
+      <c r="F238" s="49" t="s">
         <v>610</v>
       </c>
     </row>
@@ -10836,7 +10869,7 @@
       <c r="D239" t="s">
         <v>322</v>
       </c>
-      <c r="F239" s="49" t="s">
+      <c r="F239" s="48" t="s">
         <v>553</v>
       </c>
       <c r="G239" s="2" t="s">
@@ -10856,7 +10889,7 @@
       <c r="D240" t="s">
         <v>322</v>
       </c>
-      <c r="F240" s="56" t="s">
+      <c r="F240" s="55" t="s">
         <v>555</v>
       </c>
       <c r="G240" s="2" t="s">
@@ -10876,7 +10909,7 @@
       <c r="D241" t="s">
         <v>582</v>
       </c>
-      <c r="F241" s="40" t="s">
+      <c r="F241" s="39" t="s">
         <v>559</v>
       </c>
       <c r="G241" s="2" t="s">
@@ -10896,7 +10929,7 @@
       <c r="D242" t="s">
         <v>582</v>
       </c>
-      <c r="F242" s="41" t="s">
+      <c r="F242" s="40" t="s">
         <v>560</v>
       </c>
       <c r="G242" s="2" t="s">
@@ -11010,7 +11043,7 @@
       <c r="C248" t="s">
         <v>580</v>
       </c>
-      <c r="F248" s="63" t="s">
+      <c r="F248" s="35" t="s">
         <v>611</v>
       </c>
     </row>
@@ -11027,7 +11060,7 @@
       <c r="D249" t="s">
         <v>249</v>
       </c>
-      <c r="F249" s="52" t="s">
+      <c r="F249" s="51" t="s">
         <v>561</v>
       </c>
       <c r="G249" s="2" t="s">
@@ -11047,7 +11080,7 @@
       <c r="D250" t="s">
         <v>239</v>
       </c>
-      <c r="F250" s="52" t="s">
+      <c r="F250" s="51" t="s">
         <v>758</v>
       </c>
       <c r="G250" s="2" t="s">
@@ -11061,7 +11094,7 @@
       <c r="C251" t="s">
         <v>760</v>
       </c>
-      <c r="F251" s="52" t="s">
+      <c r="F251" s="51" t="s">
         <v>765</v>
       </c>
       <c r="G251" s="2"/>
@@ -11093,7 +11126,7 @@
       <c r="C253" t="s">
         <v>581</v>
       </c>
-      <c r="F253" s="52" t="s">
+      <c r="F253" s="51" t="s">
         <v>612</v>
       </c>
     </row>
@@ -11110,7 +11143,7 @@
       <c r="D254" t="s">
         <v>249</v>
       </c>
-      <c r="F254" s="52" t="s">
+      <c r="F254" s="51" t="s">
         <v>563</v>
       </c>
       <c r="G254" s="2" t="s">
@@ -11152,7 +11185,7 @@
         <v>770</v>
       </c>
       <c r="E257" s="2"/>
-      <c r="F257" s="34" t="s">
+      <c r="F257" s="2" t="s">
         <v>774</v>
       </c>
     </row>
@@ -11169,7 +11202,7 @@
       <c r="D258" t="s">
         <v>250</v>
       </c>
-      <c r="F258" s="39" t="s">
+      <c r="F258" s="38" t="s">
         <v>820</v>
       </c>
       <c r="G258" s="2" t="s">
@@ -11189,7 +11222,7 @@
       <c r="D259" t="s">
         <v>322</v>
       </c>
-      <c r="F259" s="65" t="s">
+      <c r="F259" s="63" t="s">
         <v>821</v>
       </c>
       <c r="G259" s="2" t="s">
@@ -11209,7 +11242,7 @@
       <c r="D260" t="s">
         <v>582</v>
       </c>
-      <c r="F260" s="60" t="s">
+      <c r="F260" s="59" t="s">
         <v>822</v>
       </c>
       <c r="G260" s="2" t="s">
@@ -11311,7 +11344,7 @@
       <c r="D266" t="s">
         <v>250</v>
       </c>
-      <c r="F266" s="39" t="s">
+      <c r="F266" s="38" t="s">
         <v>783</v>
       </c>
       <c r="G266" s="2" t="s">
@@ -11331,7 +11364,7 @@
       <c r="D267" t="s">
         <v>249</v>
       </c>
-      <c r="F267" s="66" t="s">
+      <c r="F267" s="64" t="s">
         <v>786</v>
       </c>
       <c r="G267" s="2" t="s">
@@ -11353,7 +11386,7 @@
       <c r="A269" t="s">
         <v>126</v>
       </c>
-      <c r="B269" s="68">
+      <c r="B269" s="66">
         <v>4</v>
       </c>
       <c r="C269" t="s">
@@ -11362,7 +11395,7 @@
       <c r="D269" t="s">
         <v>249</v>
       </c>
-      <c r="F269" s="37" t="s">
+      <c r="F269" s="36" t="s">
         <v>789</v>
       </c>
       <c r="G269" s="2" t="s">
@@ -11373,7 +11406,7 @@
       <c r="A270" t="s">
         <v>126</v>
       </c>
-      <c r="B270" s="68">
+      <c r="B270" s="66">
         <v>4</v>
       </c>
       <c r="C270" t="s">
@@ -11382,7 +11415,7 @@
       <c r="D270" t="s">
         <v>249</v>
       </c>
-      <c r="F270" s="67" t="s">
+      <c r="F270" s="65" t="s">
         <v>792</v>
       </c>
       <c r="G270" s="2" t="s">
@@ -11569,7 +11602,7 @@
       <c r="D281" t="s">
         <v>322</v>
       </c>
-      <c r="F281" s="59" t="s">
+      <c r="F281" s="58" t="s">
         <v>806</v>
       </c>
       <c r="G281" s="2" t="s">
@@ -11589,7 +11622,7 @@
       <c r="D282" t="s">
         <v>249</v>
       </c>
-      <c r="F282" s="67" t="s">
+      <c r="F282" s="65" t="s">
         <v>809</v>
       </c>
       <c r="G282" s="2" t="s">
@@ -11623,7 +11656,7 @@
       <c r="C284" t="s">
         <v>817</v>
       </c>
-      <c r="F284" s="69" t="s">
+      <c r="F284" s="67" t="s">
         <v>818</v>
       </c>
     </row>
@@ -11640,7 +11673,7 @@
       <c r="D285" t="s">
         <v>256</v>
       </c>
-      <c r="F285" s="69" t="s">
+      <c r="F285" s="67" t="s">
         <v>858</v>
       </c>
       <c r="G285" s="2" t="s">
@@ -11760,7 +11793,7 @@
       <c r="D293" t="s">
         <v>250</v>
       </c>
-      <c r="F293" s="39" t="s">
+      <c r="F293" s="38" t="s">
         <v>868</v>
       </c>
       <c r="G293" s="2" t="s">
@@ -11780,7 +11813,7 @@
       <c r="D294" t="s">
         <v>249</v>
       </c>
-      <c r="F294" s="66" t="s">
+      <c r="F294" s="64" t="s">
         <v>871</v>
       </c>
       <c r="G294" s="2" t="s">
@@ -11811,7 +11844,7 @@
       <c r="D296" t="s">
         <v>249</v>
       </c>
-      <c r="F296" s="47" t="s">
+      <c r="F296" s="46" t="s">
         <v>874</v>
       </c>
       <c r="G296" s="2" t="s">
@@ -11831,7 +11864,7 @@
       <c r="D297" t="s">
         <v>239</v>
       </c>
-      <c r="F297" s="39" t="s">
+      <c r="F297" s="38" t="s">
         <v>904</v>
       </c>
       <c r="G297" s="2" t="s">
@@ -11845,7 +11878,7 @@
       <c r="C298" t="s">
         <v>877</v>
       </c>
-      <c r="F298" s="39" t="s">
+      <c r="F298" s="38" t="s">
         <v>876</v>
       </c>
     </row>
@@ -11862,7 +11895,7 @@
       <c r="D299" t="s">
         <v>249</v>
       </c>
-      <c r="F299" s="38" t="s">
+      <c r="F299" s="37" t="s">
         <v>907</v>
       </c>
       <c r="G299" s="2" t="s">
@@ -11876,7 +11909,7 @@
       <c r="C300" t="s">
         <v>880</v>
       </c>
-      <c r="F300" s="38" t="s">
+      <c r="F300" s="37" t="s">
         <v>879</v>
       </c>
     </row>
@@ -11893,7 +11926,7 @@
       <c r="D301" t="s">
         <v>249</v>
       </c>
-      <c r="F301" s="38" t="s">
+      <c r="F301" s="37" t="s">
         <v>881</v>
       </c>
       <c r="G301" s="2" t="s">
@@ -11907,7 +11940,7 @@
       <c r="C302" t="s">
         <v>910</v>
       </c>
-      <c r="E302" s="71" t="s">
+      <c r="E302" s="69" t="s">
         <v>911</v>
       </c>
       <c r="F302" s="2" t="s">
@@ -11922,7 +11955,7 @@
       <c r="C303" t="s">
         <v>914</v>
       </c>
-      <c r="E303" s="71"/>
+      <c r="E303" s="69"/>
       <c r="F303" s="2" t="s">
         <v>913</v>
       </c>
@@ -11941,7 +11974,7 @@
       <c r="D304" t="s">
         <v>239</v>
       </c>
-      <c r="E304" s="71"/>
+      <c r="E304" s="69"/>
       <c r="F304" s="2" t="s">
         <v>915</v>
       </c>
@@ -11956,7 +11989,7 @@
       <c r="C305" t="s">
         <v>918</v>
       </c>
-      <c r="E305" s="71"/>
+      <c r="E305" s="69"/>
       <c r="F305" s="2" t="s">
         <v>919</v>
       </c>
@@ -11975,7 +12008,7 @@
       <c r="D306" t="s">
         <v>239</v>
       </c>
-      <c r="E306" s="71"/>
+      <c r="E306" s="69"/>
       <c r="F306" s="2" t="s">
         <v>921</v>
       </c>
@@ -11990,7 +12023,7 @@
       <c r="C307" t="s">
         <v>923</v>
       </c>
-      <c r="E307" s="71"/>
+      <c r="E307" s="69"/>
       <c r="F307" s="2" t="s">
         <v>924</v>
       </c>
@@ -12009,7 +12042,7 @@
       <c r="D308" t="s">
         <v>239</v>
       </c>
-      <c r="E308" s="71"/>
+      <c r="E308" s="69"/>
       <c r="F308" s="2" t="s">
         <v>925</v>
       </c>
@@ -12024,7 +12057,7 @@
       <c r="C309" t="s">
         <v>929</v>
       </c>
-      <c r="E309" s="71"/>
+      <c r="E309" s="69"/>
       <c r="F309" s="2" t="s">
         <v>928</v>
       </c>
@@ -12043,7 +12076,7 @@
       <c r="D310" t="s">
         <v>239</v>
       </c>
-      <c r="E310" s="71"/>
+      <c r="E310" s="69"/>
       <c r="F310" s="2" t="s">
         <v>930</v>
       </c>
@@ -12089,7 +12122,7 @@
       <c r="D313" t="s">
         <v>250</v>
       </c>
-      <c r="F313" s="39" t="s">
+      <c r="F313" s="38" t="s">
         <v>888</v>
       </c>
       <c r="G313" s="2" t="s">
@@ -12109,7 +12142,7 @@
       <c r="D314" t="s">
         <v>582</v>
       </c>
-      <c r="F314" s="70" t="s">
+      <c r="F314" s="68" t="s">
         <v>891</v>
       </c>
       <c r="G314" s="2" t="s">
@@ -12154,7 +12187,7 @@
       <c r="D317" t="s">
         <v>249</v>
       </c>
-      <c r="F317" s="36" t="s">
+      <c r="F317" s="35" t="s">
         <v>897</v>
       </c>
       <c r="G317" s="2" t="s">
@@ -12174,7 +12207,7 @@
       <c r="D318" t="s">
         <v>582</v>
       </c>
-      <c r="F318" s="70" t="s">
+      <c r="F318" s="68" t="s">
         <v>900</v>
       </c>
       <c r="G318" s="2" t="s">
@@ -12631,7 +12664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{242BF215-323D-D147-A6AA-4FC77FB34358}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
+    <sheetView zoomScale="168" workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix(lib): missing ID.IM-03.1 item on basic level of Cyfun 2025
</commit_message>
<xml_diff>
--- a/tools/excel/ccb/cyfun2025.xlsx
+++ b/tools/excel/ccb/cyfun2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/excel/ccb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9AE6B8-4C7B-2044-8556-59D83B060D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2082215A-E737-ED4D-BDFB-B1B64F818934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25680" yWindow="-28020" windowWidth="25360" windowHeight="27860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="-28020" windowWidth="50880" windowHeight="27860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="2" r:id="rId1"/>
@@ -6480,7 +6480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5483155-6829-0140-8BF0-A0EAE8AC9D6F}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+    <sheetView zoomScale="200" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -6511,7 +6511,7 @@
         <v>195</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -6685,9 +6685,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G335"/>
   <sheetViews>
-    <sheetView zoomScale="173" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9022,7 +9022,7 @@
         <v>429</v>
       </c>
       <c r="D136" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F136" s="36" t="s">
         <v>428</v>

</xml_diff>

<commit_message>
fix(lib): missing ID.IM-03.1 item on basic level of Cyfun 2025 (#2796)
</commit_message>
<xml_diff>
--- a/tools/excel/ccb/cyfun2025.xlsx
+++ b/tools/excel/ccb/cyfun2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/excel/ccb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9AE6B8-4C7B-2044-8556-59D83B060D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2082215A-E737-ED4D-BDFB-B1B64F818934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25680" yWindow="-28020" windowWidth="25360" windowHeight="27860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="-28020" windowWidth="50880" windowHeight="27860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="2" r:id="rId1"/>
@@ -6480,7 +6480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5483155-6829-0140-8BF0-A0EAE8AC9D6F}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+    <sheetView zoomScale="200" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -6511,7 +6511,7 @@
         <v>195</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -6685,9 +6685,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G335"/>
   <sheetViews>
-    <sheetView zoomScale="173" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9022,7 +9022,7 @@
         <v>429</v>
       </c>
       <c r="D136" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F136" s="36" t="s">
         <v>428</v>

</xml_diff>

<commit_message>
fix urn for id.am-08.10
</commit_message>
<xml_diff>
--- a/tools/excel/ccb/cyfun2025.xlsx
+++ b/tools/excel/ccb/cyfun2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/excel/ccb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9486397B-4046-9C46-836C-A21859F42ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB37660-306B-9B40-BD56-8DA48AC81C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20540" tabRatio="906" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20540" tabRatio="906" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -7051,9 +7051,6 @@
     <t xml:space="preserve">ID.AM-08.10  </t>
   </si>
   <si>
-    <t xml:space="preserve">1:ID.AM-08.10  </t>
-  </si>
-  <si>
     <t>gv.rr-03-1</t>
   </si>
   <si>
@@ -7082,6 +7079,9 @@
   </si>
   <si>
     <t xml:space="preserve">D.AM-08.10  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:D.AM-08.10  </t>
   </si>
 </sst>
 </file>
@@ -8684,7 +8684,7 @@
         <v>879</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -8912,9 +8912,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I337"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A336" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I39" sqref="I39"/>
+    <sheetView topLeftCell="H1" zoomScale="156" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I108" sqref="I108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8940,7 +8940,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="E1" s="38" t="s">
         <v>905</v>
@@ -9714,7 +9714,7 @@
         <v>1427</v>
       </c>
       <c r="D37" s="52" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>915</v>
@@ -9741,7 +9741,7 @@
         <v>1428</v>
       </c>
       <c r="D38" s="52" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>928</v>
@@ -10858,7 +10858,7 @@
         <v>1429</v>
       </c>
       <c r="D89" s="52" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="E89" s="11" t="s">
         <v>928</v>
@@ -10885,7 +10885,7 @@
         <v>1430</v>
       </c>
       <c r="D90" s="52" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="E90" s="11" t="s">
         <v>1006</v>
@@ -11305,7 +11305,7 @@
         <v>1433</v>
       </c>
       <c r="D108" s="52" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="E108" s="11" t="s">
         <v>1006</v>
@@ -11318,7 +11318,7 @@
         <v>262</v>
       </c>
       <c r="I108" s="54" t="s">
-        <v>1434</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="128" customHeight="1" x14ac:dyDescent="0.2">
@@ -14971,7 +14971,7 @@
         <v>1431</v>
       </c>
       <c r="D268" s="52" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="E268" s="11" t="s">
         <v>923</v>
@@ -14998,7 +14998,7 @@
         <v>1432</v>
       </c>
       <c r="D269" s="52" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="E269" s="11" t="s">
         <v>928</v>
@@ -16520,9 +16520,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E219"/>
   <sheetViews>
-    <sheetView zoomScale="184" zoomScaleNormal="119" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B182" sqref="B182"/>
+    <sheetView tabSelected="1" zoomScale="184" zoomScaleNormal="119" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16538,7 +16538,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>1</v>
@@ -17523,7 +17523,7 @@
         <v>1433</v>
       </c>
       <c r="B66" s="56" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="C66" s="11" t="s">
         <v>260</v>

</xml_diff>